<commit_message>
added consumerfunction to main.m
Now the CONSUMPTION file is unnecessary, all is generated from the meta file and the E_c is created with the consumerFunction
</commit_message>
<xml_diff>
--- a/META.xlsx
+++ b/META.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2EF3A-B5A8-451F-92A9-DDF3855D310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C9C4F6-FBA6-4C09-901B-0DB75186084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>Variable</t>
   </si>
@@ -115,10 +115,16 @@
     <t>DC line</t>
   </si>
   <si>
-    <t>residential</t>
-  </si>
-  <si>
-    <t>commercial</t>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>residential_-5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>commercial_-8</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E19" sqref="E19:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +482,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -485,15 +491,15 @@
         <v>25</v>
       </c>
       <c r="E2">
-        <v>52.343337996743898</v>
+        <v>43.6</v>
       </c>
       <c r="F2">
-        <v>4.9358207840021304</v>
+        <v>-116.2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -502,15 +508,15 @@
         <v>25</v>
       </c>
       <c r="E3">
-        <v>52.119578270165398</v>
+        <v>43.5</v>
       </c>
       <c r="F3">
-        <v>6.4025977569452204</v>
+        <v>-115.3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -519,15 +525,15 @@
         <v>25</v>
       </c>
       <c r="E4">
-        <v>52.592887648614301</v>
+        <v>51.6189802813036</v>
       </c>
       <c r="F4">
-        <v>4.0988236582999997</v>
+        <v>5.71901122838461</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -536,15 +542,15 @@
         <v>25</v>
       </c>
       <c r="E5">
-        <v>51.6189802813036</v>
+        <v>51.5</v>
       </c>
       <c r="F5">
-        <v>5.71901122838461</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -561,7 +567,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -570,37 +576,49 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>53.198799420490097</v>
+        <v>51.8902154304227</v>
       </c>
       <c r="F7">
-        <v>6.5688442594149397</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>52.343337996743898</v>
+      </c>
+      <c r="F8">
+        <v>4.9358207840021304</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>53.198799420490097</v>
+      </c>
+      <c r="F9">
+        <v>6.5688442594149397</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -611,108 +629,84 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="1">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="1">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="1">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="1">
-        <v>90</v>
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -723,52 +717,64 @@
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18">
-        <v>10</v>
+      <c r="E18" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19">
-        <v>0.997</v>
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21">
-        <v>0.98499999999999999</v>
+        <v>26</v>
+      </c>
+      <c r="E21" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -776,89 +782,182 @@
       <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="E22">
-        <v>20</v>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23">
-        <v>23.45</v>
+        <v>26</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E24">
-        <v>0.42370000000000002</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E25">
-        <v>0.50549999999999995</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30">
+        <v>0.42370000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>0.50549999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
         <v>22</v>
       </c>
-      <c r="E26">
+      <c r="E32">
         <v>0.27110000000000001</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="1"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E59" s="1"/>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a lot of data to META (hydro, hydrogen, ammonia). Modified code to be able to provide flat distributions of energy
</commit_message>
<xml_diff>
--- a/META.xlsx
+++ b/META.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AB6D1B-83BA-4F42-881A-4A351036D381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0469B8B-C4E6-4AFA-A857-03D2CD6CC983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1524" yWindow="792" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="134">
   <si>
     <t>Variable</t>
   </si>
@@ -295,13 +295,154 @@
   </si>
   <si>
     <t>commercial_-8</t>
+  </si>
+  <si>
+    <t>c21</t>
+  </si>
+  <si>
+    <t>c22</t>
+  </si>
+  <si>
+    <t>c23</t>
+  </si>
+  <si>
+    <t>c24</t>
+  </si>
+  <si>
+    <t>c25</t>
+  </si>
+  <si>
+    <t>c26</t>
+  </si>
+  <si>
+    <t>c27</t>
+  </si>
+  <si>
+    <t>c28</t>
+  </si>
+  <si>
+    <t>c29</t>
+  </si>
+  <si>
+    <t>c30</t>
+  </si>
+  <si>
+    <t>c31</t>
+  </si>
+  <si>
+    <t>c32</t>
+  </si>
+  <si>
+    <t>c33</t>
+  </si>
+  <si>
+    <t>c34</t>
+  </si>
+  <si>
+    <t>c35</t>
+  </si>
+  <si>
+    <t>c36</t>
+  </si>
+  <si>
+    <t>c37</t>
+  </si>
+  <si>
+    <t>c38</t>
+  </si>
+  <si>
+    <t>c39</t>
+  </si>
+  <si>
+    <t>c40</t>
+  </si>
+  <si>
+    <t>industrial_-7</t>
+  </si>
+  <si>
+    <t>industrial_-6</t>
+  </si>
+  <si>
+    <t>industrial_-5</t>
+  </si>
+  <si>
+    <t>industrial_-8</t>
+  </si>
+  <si>
+    <t>transportation_-7</t>
+  </si>
+  <si>
+    <t>transportation_-6</t>
+  </si>
+  <si>
+    <t>transportation_-5</t>
+  </si>
+  <si>
+    <t>transportation_-8</t>
+  </si>
+  <si>
+    <t>p24</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p26</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>p27</t>
+  </si>
+  <si>
+    <t>p28</t>
+  </si>
+  <si>
+    <t>p29</t>
+  </si>
+  <si>
+    <t>c41</t>
+  </si>
+  <si>
+    <t>c42</t>
+  </si>
+  <si>
+    <t>c43</t>
+  </si>
+  <si>
+    <t>c44</t>
+  </si>
+  <si>
+    <t>c45</t>
+  </si>
+  <si>
+    <t>c46</t>
+  </si>
+  <si>
+    <t>c47</t>
+  </si>
+  <si>
+    <t>c48</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>c49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +455,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,15 +485,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{C6E5397D-20AA-4F8D-AC05-8671B1DB7801}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -619,15 +782,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F185"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="E248" sqref="E248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -692,7 +857,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -737,7 +902,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -782,7 +947,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -827,7 +992,7 @@
         <v>24</v>
       </c>
       <c r="E13" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -872,7 +1037,7 @@
         <v>24</v>
       </c>
       <c r="E16" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -917,7 +1082,7 @@
         <v>24</v>
       </c>
       <c r="E19" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -962,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1007,7 +1172,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1052,7 +1217,7 @@
         <v>24</v>
       </c>
       <c r="E28" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,7 +1262,7 @@
         <v>24</v>
       </c>
       <c r="E31" s="1">
-        <v>30</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1160,7 +1325,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="1">
-        <v>25.07</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1205,7 +1370,7 @@
         <v>24</v>
       </c>
       <c r="E40" s="1">
-        <v>31.44</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1250,7 +1415,7 @@
         <v>24</v>
       </c>
       <c r="E43" s="1">
-        <v>37.28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1295,7 +1460,7 @@
         <v>24</v>
       </c>
       <c r="E46" s="1">
-        <v>26.25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1340,7 +1505,7 @@
         <v>24</v>
       </c>
       <c r="E49" s="1">
-        <v>39.119999999999997</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1385,7 +1550,7 @@
         <v>24</v>
       </c>
       <c r="E52" s="1">
-        <v>25.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,7 +1595,7 @@
         <v>24</v>
       </c>
       <c r="E55" s="1">
-        <v>26.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1475,7 +1640,7 @@
         <v>24</v>
       </c>
       <c r="E58" s="1">
-        <v>31.15</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1520,7 +1685,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="1">
-        <v>25.54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1565,7 +1730,7 @@
         <v>24</v>
       </c>
       <c r="E64" s="1">
-        <v>47.56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1610,7 +1775,7 @@
         <v>24</v>
       </c>
       <c r="E67" s="1">
-        <v>17.190000000000001</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1655,7 +1820,7 @@
         <v>24</v>
       </c>
       <c r="E70" s="1">
-        <v>32.049999999999997</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1700,309 +1865,309 @@
         <v>24</v>
       </c>
       <c r="E73" s="1">
-        <v>47.16</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>32</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="2">
+        <v>47.751075999999998</v>
+      </c>
+      <c r="F74" s="2">
+        <v>-120.740135</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>32</v>
-      </c>
-      <c r="E75" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>32</v>
+        <v>116</v>
+      </c>
+      <c r="B76" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="1">
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>32</v>
+        <v>117</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="4">
+        <v>36.778258999999998</v>
+      </c>
+      <c r="F77" s="4">
+        <v>-119.417931</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>32</v>
+        <v>117</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>23</v>
-      </c>
-      <c r="E79">
-        <v>43.615000000000002</v>
-      </c>
-      <c r="F79">
-        <v>-116.2</v>
+        <v>24</v>
+      </c>
+      <c r="E79" s="1">
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" t="s">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="5">
+        <v>44</v>
+      </c>
+      <c r="F80" s="5">
+        <v>-120.5</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81">
-        <v>74.16</v>
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82">
-        <v>41.87</v>
-      </c>
-      <c r="F82">
-        <v>-87.63</v>
+        <v>24</v>
+      </c>
+      <c r="E82" s="1">
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" t="s">
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" s="6">
+        <v>43</v>
+      </c>
+      <c r="F83" s="6">
+        <v>-75</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" t="s">
-        <v>24</v>
-      </c>
-      <c r="E84">
-        <v>120.72</v>
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>23</v>
-      </c>
-      <c r="E85">
-        <v>40.71</v>
-      </c>
-      <c r="F85">
-        <v>-74</v>
+        <v>24</v>
+      </c>
+      <c r="E85" s="1">
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="8">
+        <v>32.31823</v>
+      </c>
+      <c r="F86" s="7">
+        <v>-86.902298000000002</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="B87" t="s">
-        <v>13</v>
-      </c>
-      <c r="C87" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" t="s">
-        <v>24</v>
-      </c>
-      <c r="E87">
-        <v>134.88999999999999</v>
+        <v>11</v>
+      </c>
+      <c r="E87" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>23</v>
-      </c>
-      <c r="E88">
-        <v>33.75</v>
-      </c>
-      <c r="F88">
-        <v>-84.38</v>
+        <v>24</v>
+      </c>
+      <c r="E88" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" t="s">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="9">
+        <v>21.167635000000001</v>
+      </c>
+      <c r="F89" s="9">
+        <v>-105.22829400000001</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90">
-        <v>125.4</v>
+        <v>11</v>
+      </c>
+      <c r="E90" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C91" t="s">
+        <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>23</v>
-      </c>
-      <c r="E91">
-        <v>36.159999999999997</v>
-      </c>
-      <c r="F91">
-        <v>-86.78</v>
+        <v>24</v>
+      </c>
+      <c r="E91" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>37</v>
-      </c>
-      <c r="B92" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>37</v>
-      </c>
-      <c r="B93" t="s">
-        <v>13</v>
-      </c>
-      <c r="C93" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93">
-        <v>81.599999999999994</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>38</v>
-      </c>
-      <c r="B94" t="s">
-        <v>4</v>
-      </c>
-      <c r="D94" t="s">
-        <v>23</v>
-      </c>
-      <c r="E94">
-        <v>30.26</v>
-      </c>
-      <c r="F94">
-        <v>-97.74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>38</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
-      </c>
-      <c r="E95" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>38</v>
-      </c>
-      <c r="B96" t="s">
-        <v>13</v>
-      </c>
-      <c r="C96" t="s">
-        <v>14</v>
-      </c>
-      <c r="D96" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96">
-        <v>87.19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B97" t="s">
         <v>4</v>
@@ -2011,26 +2176,26 @@
         <v>23</v>
       </c>
       <c r="E97">
-        <v>38.58</v>
+        <v>43.615000000000002</v>
       </c>
       <c r="F97">
-        <v>-121.49</v>
+        <v>-116.2</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
         <v>11</v>
       </c>
       <c r="E98" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B99" t="s">
         <v>13</v>
@@ -2042,12 +2207,12 @@
         <v>24</v>
       </c>
       <c r="E99">
-        <v>80.209999999999994</v>
+        <v>74.16</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
         <v>4</v>
@@ -2056,15 +2221,15 @@
         <v>23</v>
       </c>
       <c r="E100">
-        <v>20.68</v>
+        <v>41.87</v>
       </c>
       <c r="F100">
-        <v>-103.34</v>
+        <v>-87.63</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B101" t="s">
         <v>11</v>
@@ -2075,7 +2240,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
         <v>13</v>
@@ -2087,12 +2252,12 @@
         <v>24</v>
       </c>
       <c r="E102">
-        <v>10.62</v>
+        <v>120.72</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B103" t="s">
         <v>4</v>
@@ -2101,26 +2266,26 @@
         <v>23</v>
       </c>
       <c r="E103">
-        <v>19.43</v>
+        <v>40.71</v>
       </c>
       <c r="F103">
-        <v>-99.13</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B104" t="s">
         <v>11</v>
       </c>
       <c r="E104" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B105" t="s">
         <v>13</v>
@@ -2132,12 +2297,12 @@
         <v>24</v>
       </c>
       <c r="E105">
-        <v>10.62</v>
+        <v>134.88999999999999</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B106" t="s">
         <v>4</v>
@@ -2146,26 +2311,26 @@
         <v>23</v>
       </c>
       <c r="E106">
-        <v>19.04</v>
+        <v>33.75</v>
       </c>
       <c r="F106">
-        <v>-98.19</v>
+        <v>-84.38</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B107" t="s">
         <v>11</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B108" t="s">
         <v>13</v>
@@ -2177,287 +2342,287 @@
         <v>24</v>
       </c>
       <c r="E108">
-        <v>10.62</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" t="s">
+        <v>23</v>
+      </c>
+      <c r="E109">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="F109">
+        <v>-86.78</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
-      </c>
-      <c r="D110" t="s">
-        <v>23</v>
-      </c>
-      <c r="E110">
-        <v>43.615000000000002</v>
-      </c>
-      <c r="F110">
-        <v>-116.2</v>
+        <v>11</v>
+      </c>
+      <c r="E110" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B111" t="s">
-        <v>11</v>
-      </c>
-      <c r="E111" t="s">
-        <v>84</v>
+        <v>13</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111">
+        <v>81.599999999999994</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
-      </c>
-      <c r="C112" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E112">
-        <v>60.3</v>
+        <v>30.26</v>
+      </c>
+      <c r="F112">
+        <v>-97.74</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
-      </c>
-      <c r="D113" t="s">
-        <v>23</v>
-      </c>
-      <c r="E113">
-        <v>41.87</v>
-      </c>
-      <c r="F113">
-        <v>-87.63</v>
+        <v>11</v>
+      </c>
+      <c r="E113" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B114" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" t="s">
-        <v>85</v>
+        <v>13</v>
+      </c>
+      <c r="C114" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" t="s">
+        <v>24</v>
+      </c>
+      <c r="E114">
+        <v>87.19</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
-      </c>
-      <c r="C115" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E115">
-        <v>90.295000000000002</v>
+        <v>38.58</v>
+      </c>
+      <c r="F115">
+        <v>-121.49</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
-      </c>
-      <c r="D116" t="s">
-        <v>23</v>
-      </c>
-      <c r="E116">
-        <v>40.71</v>
-      </c>
-      <c r="F116">
-        <v>-74</v>
+        <v>11</v>
+      </c>
+      <c r="E116" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
-      </c>
-      <c r="E117" t="s">
-        <v>86</v>
+        <v>13</v>
+      </c>
+      <c r="C117" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" t="s">
+        <v>24</v>
+      </c>
+      <c r="E117">
+        <v>80.209999999999994</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>13</v>
-      </c>
-      <c r="C118" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E118">
-        <v>113.67</v>
+        <v>20.68</v>
+      </c>
+      <c r="F118">
+        <v>-103.34</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
-      </c>
-      <c r="D119" t="s">
-        <v>23</v>
-      </c>
-      <c r="E119">
-        <v>33.75</v>
-      </c>
-      <c r="F119">
-        <v>-84.38</v>
+        <v>11</v>
+      </c>
+      <c r="E119" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
-      </c>
-      <c r="E120" t="s">
-        <v>86</v>
+        <v>13</v>
+      </c>
+      <c r="C120" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" t="s">
+        <v>24</v>
+      </c>
+      <c r="E120">
+        <v>10.62</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
-      </c>
-      <c r="C121" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E121">
-        <v>100.289</v>
+        <v>19.43</v>
+      </c>
+      <c r="F121">
+        <v>-99.13</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
-      </c>
-      <c r="D122" t="s">
-        <v>23</v>
-      </c>
-      <c r="E122">
-        <v>36.159999999999997</v>
-      </c>
-      <c r="F122">
-        <v>-86.78</v>
+        <v>11</v>
+      </c>
+      <c r="E122" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="B123" t="s">
-        <v>11</v>
-      </c>
-      <c r="E123" t="s">
-        <v>85</v>
+        <v>13</v>
+      </c>
+      <c r="C123" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123">
+        <v>10.62</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B124" t="s">
-        <v>13</v>
-      </c>
-      <c r="C124" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D124" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E124">
-        <v>62.23</v>
+        <v>19.04</v>
+      </c>
+      <c r="F124">
+        <v>-98.19</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
-      </c>
-      <c r="D125" t="s">
-        <v>23</v>
-      </c>
-      <c r="E125">
-        <v>30.26</v>
-      </c>
-      <c r="F125">
-        <v>-97.74</v>
+        <v>11</v>
+      </c>
+      <c r="E125" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B126" t="s">
-        <v>11</v>
-      </c>
-      <c r="E126" t="s">
-        <v>85</v>
+        <v>13</v>
+      </c>
+      <c r="C126" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" t="s">
+        <v>24</v>
+      </c>
+      <c r="E126">
+        <v>10.62</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>79</v>
-      </c>
-      <c r="B127" t="s">
-        <v>13</v>
-      </c>
-      <c r="C127" t="s">
-        <v>14</v>
-      </c>
-      <c r="D127" t="s">
-        <v>24</v>
-      </c>
-      <c r="E127">
-        <v>77.58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B128" t="s">
         <v>4</v>
@@ -2466,26 +2631,26 @@
         <v>23</v>
       </c>
       <c r="E128">
-        <v>38.58</v>
+        <v>43.615000000000002</v>
       </c>
       <c r="F128">
-        <v>-121.49</v>
+        <v>-116.2</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B129" t="s">
         <v>11</v>
       </c>
       <c r="E129" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B130" t="s">
         <v>13</v>
@@ -2497,12 +2662,12 @@
         <v>24</v>
       </c>
       <c r="E130">
-        <v>69.209999999999994</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B131" t="s">
         <v>4</v>
@@ -2511,15 +2676,15 @@
         <v>23</v>
       </c>
       <c r="E131">
-        <v>20.68</v>
+        <v>41.87</v>
       </c>
       <c r="F131">
-        <v>-103.34</v>
+        <v>-87.63</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B132" t="s">
         <v>11</v>
@@ -2530,7 +2695,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B133" t="s">
         <v>13</v>
@@ -2542,12 +2707,12 @@
         <v>24</v>
       </c>
       <c r="E133">
-        <v>2.65</v>
+        <v>90.295000000000002</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B134" t="s">
         <v>4</v>
@@ -2556,26 +2721,26 @@
         <v>23</v>
       </c>
       <c r="E134">
-        <v>19.43</v>
+        <v>40.71</v>
       </c>
       <c r="F134">
-        <v>-99.13</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B135" t="s">
         <v>11</v>
       </c>
       <c r="E135" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B136" t="s">
         <v>13</v>
@@ -2587,12 +2752,12 @@
         <v>24</v>
       </c>
       <c r="E136">
-        <v>2.65</v>
+        <v>113.67</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B137" t="s">
         <v>4</v>
@@ -2601,26 +2766,26 @@
         <v>23</v>
       </c>
       <c r="E137">
-        <v>19.04</v>
+        <v>33.75</v>
       </c>
       <c r="F137">
-        <v>-98.19</v>
+        <v>-84.38</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B138" t="s">
         <v>11</v>
       </c>
       <c r="E138" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B139" t="s">
         <v>13</v>
@@ -2632,185 +2797,1715 @@
         <v>24</v>
       </c>
       <c r="E139">
-        <v>2.65</v>
+        <v>100.289</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>23</v>
+      </c>
+      <c r="E140">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="F140">
+        <v>-86.78</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="B141" t="s">
+        <v>11</v>
+      </c>
+      <c r="E141" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="B142" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142">
+        <v>62.23</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>32</v>
+        <v>79</v>
+      </c>
+      <c r="B143" t="s">
+        <v>4</v>
+      </c>
+      <c r="D143" t="s">
+        <v>23</v>
+      </c>
+      <c r="E143">
+        <v>30.26</v>
+      </c>
+      <c r="F143">
+        <v>-97.74</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>79</v>
+      </c>
+      <c r="B144" t="s">
+        <v>11</v>
+      </c>
+      <c r="E144" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>79</v>
+      </c>
+      <c r="B145" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" t="s">
+        <v>24</v>
+      </c>
+      <c r="E145">
+        <v>77.58</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="D146" t="s">
+        <v>23</v>
+      </c>
+      <c r="E146">
+        <v>38.58</v>
+      </c>
+      <c r="F146">
+        <v>-121.49</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>80</v>
+      </c>
+      <c r="B147" t="s">
+        <v>11</v>
+      </c>
+      <c r="E147" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>80</v>
+      </c>
+      <c r="B148" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" t="s">
+        <v>24</v>
+      </c>
+      <c r="E148">
+        <v>69.209999999999994</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>81</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="D149" t="s">
+        <v>23</v>
+      </c>
+      <c r="E149">
+        <v>20.68</v>
+      </c>
+      <c r="F149">
+        <v>-103.34</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>81</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+      <c r="E150" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>81</v>
+      </c>
+      <c r="B151" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" t="s">
+        <v>24</v>
+      </c>
+      <c r="E151">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>82</v>
+      </c>
+      <c r="B152" t="s">
+        <v>4</v>
+      </c>
+      <c r="D152" t="s">
+        <v>23</v>
+      </c>
+      <c r="E152">
+        <v>19.43</v>
+      </c>
+      <c r="F152">
+        <v>-99.13</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>82</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="E153" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>82</v>
+      </c>
+      <c r="B154" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" t="s">
+        <v>24</v>
+      </c>
+      <c r="E154">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>83</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" t="s">
+        <v>23</v>
+      </c>
+      <c r="E155">
+        <v>19.04</v>
+      </c>
+      <c r="F155">
+        <v>-98.19</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>83</v>
+      </c>
+      <c r="B156" t="s">
+        <v>11</v>
+      </c>
+      <c r="E156" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>83</v>
+      </c>
+      <c r="B157" t="s">
+        <v>13</v>
+      </c>
+      <c r="C157" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" t="s">
+        <v>24</v>
+      </c>
+      <c r="E157">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>88</v>
+      </c>
+      <c r="B160" t="s">
+        <v>4</v>
+      </c>
+      <c r="D160" t="s">
+        <v>23</v>
+      </c>
+      <c r="E160">
+        <v>43.615000000000002</v>
+      </c>
+      <c r="F160">
+        <v>-116.2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>88</v>
+      </c>
+      <c r="B161" t="s">
+        <v>11</v>
+      </c>
+      <c r="E161" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>88</v>
+      </c>
+      <c r="B162" t="s">
+        <v>13</v>
+      </c>
+      <c r="C162" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" t="s">
+        <v>24</v>
+      </c>
+      <c r="E162">
+        <v>83.14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>89</v>
+      </c>
+      <c r="B163" t="s">
+        <v>4</v>
+      </c>
+      <c r="D163" t="s">
+        <v>23</v>
+      </c>
+      <c r="E163">
+        <v>41.87</v>
+      </c>
+      <c r="F163">
+        <v>-87.63</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>89</v>
+      </c>
+      <c r="B164" t="s">
+        <v>11</v>
+      </c>
+      <c r="E164" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>89</v>
+      </c>
+      <c r="B165" t="s">
+        <v>13</v>
+      </c>
+      <c r="C165" t="s">
+        <v>14</v>
+      </c>
+      <c r="D165" t="s">
+        <v>24</v>
+      </c>
+      <c r="E165">
+        <v>94.47</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>90</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" t="s">
+        <v>23</v>
+      </c>
+      <c r="E166">
+        <v>40.71</v>
+      </c>
+      <c r="F166">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>90</v>
+      </c>
+      <c r="B167" t="s">
+        <v>11</v>
+      </c>
+      <c r="E167" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>90</v>
+      </c>
+      <c r="B168" t="s">
+        <v>13</v>
+      </c>
+      <c r="C168" t="s">
+        <v>14</v>
+      </c>
+      <c r="D168" t="s">
+        <v>24</v>
+      </c>
+      <c r="E168">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>91</v>
+      </c>
+      <c r="B169" t="s">
+        <v>4</v>
+      </c>
+      <c r="D169" t="s">
+        <v>23</v>
+      </c>
+      <c r="E169">
+        <v>33.75</v>
+      </c>
+      <c r="F169">
+        <v>-84.38</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>91</v>
+      </c>
+      <c r="B170" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>91</v>
+      </c>
+      <c r="B171" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" t="s">
+        <v>24</v>
+      </c>
+      <c r="E171">
+        <v>61.74</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>92</v>
+      </c>
+      <c r="B172" t="s">
+        <v>4</v>
+      </c>
+      <c r="D172" t="s">
+        <v>23</v>
+      </c>
+      <c r="E172">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="F172">
+        <v>-86.78</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>92</v>
+      </c>
+      <c r="B173" t="s">
+        <v>11</v>
+      </c>
+      <c r="E173" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>92</v>
+      </c>
+      <c r="B174" t="s">
+        <v>13</v>
+      </c>
+      <c r="C174" t="s">
+        <v>14</v>
+      </c>
+      <c r="D174" t="s">
+        <v>24</v>
+      </c>
+      <c r="E174">
+        <v>123.27</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>93</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" t="s">
+        <v>23</v>
+      </c>
+      <c r="E175">
+        <v>30.26</v>
+      </c>
+      <c r="F175">
+        <v>-97.74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>93</v>
+      </c>
+      <c r="B176" t="s">
+        <v>11</v>
+      </c>
+      <c r="E176" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>93</v>
+      </c>
+      <c r="B177" t="s">
+        <v>13</v>
+      </c>
+      <c r="C177" t="s">
+        <v>14</v>
+      </c>
+      <c r="D177" t="s">
+        <v>24</v>
+      </c>
+      <c r="E177">
+        <v>176.7</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>94</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>23</v>
+      </c>
+      <c r="E178">
+        <v>38.58</v>
+      </c>
+      <c r="F178">
+        <v>-121.49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>94</v>
+      </c>
+      <c r="B179" t="s">
+        <v>11</v>
+      </c>
+      <c r="E179" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>94</v>
+      </c>
+      <c r="B180" t="s">
+        <v>13</v>
+      </c>
+      <c r="C180" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" t="s">
+        <v>24</v>
+      </c>
+      <c r="E180">
+        <v>47.37</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>95</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4</v>
+      </c>
+      <c r="D181" t="s">
+        <v>23</v>
+      </c>
+      <c r="E181">
+        <v>20.68</v>
+      </c>
+      <c r="F181">
+        <v>-103.34</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>95</v>
+      </c>
+      <c r="B182" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>95</v>
+      </c>
+      <c r="B183" t="s">
+        <v>13</v>
+      </c>
+      <c r="C183" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" t="s">
+        <v>24</v>
+      </c>
+      <c r="E183">
+        <v>10.64</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>96</v>
+      </c>
+      <c r="B184" t="s">
+        <v>4</v>
+      </c>
+      <c r="D184" t="s">
+        <v>23</v>
+      </c>
+      <c r="E184">
+        <v>19.43</v>
+      </c>
+      <c r="F184">
+        <v>-99.13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>96</v>
+      </c>
+      <c r="B185" t="s">
+        <v>11</v>
+      </c>
+      <c r="E185" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>96</v>
+      </c>
+      <c r="B186" t="s">
+        <v>13</v>
+      </c>
+      <c r="C186" t="s">
+        <v>14</v>
+      </c>
+      <c r="D186" t="s">
+        <v>24</v>
+      </c>
+      <c r="E186">
+        <v>10.64</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>97</v>
+      </c>
+      <c r="B187" t="s">
+        <v>4</v>
+      </c>
+      <c r="D187" t="s">
+        <v>23</v>
+      </c>
+      <c r="E187">
+        <v>19.04</v>
+      </c>
+      <c r="F187">
+        <v>-98.19</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>97</v>
+      </c>
+      <c r="B188" t="s">
+        <v>11</v>
+      </c>
+      <c r="E188" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>97</v>
+      </c>
+      <c r="B189" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" t="s">
+        <v>14</v>
+      </c>
+      <c r="D189" t="s">
+        <v>24</v>
+      </c>
+      <c r="E189">
+        <v>10.64</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>98</v>
+      </c>
+      <c r="B191" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>23</v>
+      </c>
+      <c r="E191">
+        <v>43.615000000000002</v>
+      </c>
+      <c r="F191">
+        <v>-116.2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>98</v>
+      </c>
+      <c r="B192" t="s">
+        <v>11</v>
+      </c>
+      <c r="E192" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>98</v>
+      </c>
+      <c r="B193" t="s">
+        <v>13</v>
+      </c>
+      <c r="C193" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" t="s">
+        <v>24</v>
+      </c>
+      <c r="E193">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>99</v>
+      </c>
+      <c r="B194" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" t="s">
+        <v>23</v>
+      </c>
+      <c r="E194">
+        <v>41.87</v>
+      </c>
+      <c r="F194">
+        <v>-87.63</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>99</v>
+      </c>
+      <c r="B195" t="s">
+        <v>11</v>
+      </c>
+      <c r="E195" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>99</v>
+      </c>
+      <c r="B196" t="s">
+        <v>13</v>
+      </c>
+      <c r="C196" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" t="s">
+        <v>24</v>
+      </c>
+      <c r="E196">
+        <v>83.28</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>100</v>
+      </c>
+      <c r="B197" t="s">
+        <v>4</v>
+      </c>
+      <c r="D197" t="s">
+        <v>23</v>
+      </c>
+      <c r="E197">
+        <v>40.71</v>
+      </c>
+      <c r="F197">
+        <v>-74</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>100</v>
+      </c>
+      <c r="B198" t="s">
+        <v>11</v>
+      </c>
+      <c r="E198" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>100</v>
+      </c>
+      <c r="B199" t="s">
+        <v>13</v>
+      </c>
+      <c r="C199" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" t="s">
+        <v>24</v>
+      </c>
+      <c r="E199">
+        <v>93.2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>101</v>
+      </c>
+      <c r="B200" t="s">
+        <v>4</v>
+      </c>
+      <c r="D200" t="s">
+        <v>23</v>
+      </c>
+      <c r="E200">
+        <v>33.75</v>
+      </c>
+      <c r="F200">
+        <v>-84.38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>101</v>
+      </c>
+      <c r="B201" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>101</v>
+      </c>
+      <c r="B202" t="s">
+        <v>13</v>
+      </c>
+      <c r="C202" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" t="s">
+        <v>24</v>
+      </c>
+      <c r="E202">
+        <v>111.24</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>102</v>
+      </c>
+      <c r="B203" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" t="s">
+        <v>23</v>
+      </c>
+      <c r="E203">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="F203">
+        <v>-86.78</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>102</v>
+      </c>
+      <c r="B204" t="s">
+        <v>11</v>
+      </c>
+      <c r="E204" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>102</v>
+      </c>
+      <c r="B205" t="s">
+        <v>13</v>
+      </c>
+      <c r="C205" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" t="s">
+        <v>24</v>
+      </c>
+      <c r="E205">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>103</v>
+      </c>
+      <c r="B206" t="s">
+        <v>4</v>
+      </c>
+      <c r="D206" t="s">
+        <v>23</v>
+      </c>
+      <c r="E206">
+        <v>30.26</v>
+      </c>
+      <c r="F206">
+        <v>-97.74</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>103</v>
+      </c>
+      <c r="B207" t="s">
+        <v>11</v>
+      </c>
+      <c r="E207" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>103</v>
+      </c>
+      <c r="B208" t="s">
+        <v>13</v>
+      </c>
+      <c r="C208" t="s">
+        <v>14</v>
+      </c>
+      <c r="D208" t="s">
+        <v>24</v>
+      </c>
+      <c r="E208">
+        <v>100.58</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>104</v>
+      </c>
+      <c r="B209" t="s">
+        <v>4</v>
+      </c>
+      <c r="D209" t="s">
+        <v>23</v>
+      </c>
+      <c r="E209">
+        <v>38.58</v>
+      </c>
+      <c r="F209">
+        <v>-121.49</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>104</v>
+      </c>
+      <c r="B210" t="s">
+        <v>11</v>
+      </c>
+      <c r="E210" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>104</v>
+      </c>
+      <c r="B211" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211" t="s">
+        <v>14</v>
+      </c>
+      <c r="D211" t="s">
+        <v>24</v>
+      </c>
+      <c r="E211">
+        <v>87.02</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>105</v>
+      </c>
+      <c r="B212" t="s">
+        <v>4</v>
+      </c>
+      <c r="D212" t="s">
+        <v>23</v>
+      </c>
+      <c r="E212">
+        <v>20.68</v>
+      </c>
+      <c r="F212">
+        <v>-103.34</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>105</v>
+      </c>
+      <c r="B213" t="s">
+        <v>11</v>
+      </c>
+      <c r="E213" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>105</v>
+      </c>
+      <c r="B214" t="s">
+        <v>13</v>
+      </c>
+      <c r="C214" t="s">
+        <v>14</v>
+      </c>
+      <c r="D214" t="s">
+        <v>24</v>
+      </c>
+      <c r="E214">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>106</v>
+      </c>
+      <c r="B215" t="s">
+        <v>4</v>
+      </c>
+      <c r="D215" t="s">
+        <v>23</v>
+      </c>
+      <c r="E215">
+        <v>19.43</v>
+      </c>
+      <c r="F215">
+        <v>-99.13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>106</v>
+      </c>
+      <c r="B216" t="s">
+        <v>11</v>
+      </c>
+      <c r="E216" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>106</v>
+      </c>
+      <c r="B217" t="s">
+        <v>13</v>
+      </c>
+      <c r="C217" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" t="s">
+        <v>24</v>
+      </c>
+      <c r="E217">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>107</v>
+      </c>
+      <c r="B218" t="s">
+        <v>4</v>
+      </c>
+      <c r="D218" t="s">
+        <v>23</v>
+      </c>
+      <c r="E218">
+        <v>19.04</v>
+      </c>
+      <c r="F218">
+        <v>-98.19</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>107</v>
+      </c>
+      <c r="B219" t="s">
+        <v>11</v>
+      </c>
+      <c r="E219" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>107</v>
+      </c>
+      <c r="B220" t="s">
+        <v>13</v>
+      </c>
+      <c r="C220" t="s">
+        <v>14</v>
+      </c>
+      <c r="D220" t="s">
+        <v>24</v>
+      </c>
+      <c r="E220">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>123</v>
+      </c>
+      <c r="B222" t="s">
+        <v>4</v>
+      </c>
+      <c r="D222" t="s">
+        <v>23</v>
+      </c>
+      <c r="E222" s="3">
+        <v>36.778258999999998</v>
+      </c>
+      <c r="F222" s="3">
+        <v>-119.417931</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>123</v>
+      </c>
+      <c r="B223" t="s">
+        <v>11</v>
+      </c>
+      <c r="E223" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>123</v>
+      </c>
+      <c r="B224" t="s">
+        <v>13</v>
+      </c>
+      <c r="C224" t="s">
+        <v>14</v>
+      </c>
+      <c r="D224" t="s">
+        <v>24</v>
+      </c>
+      <c r="E224">
+        <v>221.14</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>124</v>
+      </c>
+      <c r="B225" t="s">
+        <v>4</v>
+      </c>
+      <c r="D225" t="s">
+        <v>23</v>
+      </c>
+      <c r="E225" s="10">
+        <v>30.391829999999999</v>
+      </c>
+      <c r="F225" s="3">
+        <v>-92.329102000000006</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>124</v>
+      </c>
+      <c r="B226" t="s">
+        <v>11</v>
+      </c>
+      <c r="E226" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>124</v>
+      </c>
+      <c r="B227" t="s">
+        <v>13</v>
+      </c>
+      <c r="C227" t="s">
+        <v>14</v>
+      </c>
+      <c r="D227" t="s">
+        <v>24</v>
+      </c>
+      <c r="E227">
+        <v>70.02</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>125</v>
+      </c>
+      <c r="B228" t="s">
+        <v>4</v>
+      </c>
+      <c r="D228" t="s">
+        <v>23</v>
+      </c>
+      <c r="E228" s="10">
+        <v>31</v>
+      </c>
+      <c r="F228" s="10">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>125</v>
+      </c>
+      <c r="B229" t="s">
+        <v>11</v>
+      </c>
+      <c r="E229" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>125</v>
+      </c>
+      <c r="B230" t="s">
+        <v>13</v>
+      </c>
+      <c r="C230" t="s">
+        <v>14</v>
+      </c>
+      <c r="D230" t="s">
+        <v>24</v>
+      </c>
+      <c r="E230">
+        <v>273.76</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>126</v>
+      </c>
+      <c r="B231" t="s">
+        <v>4</v>
+      </c>
+      <c r="D231" t="s">
+        <v>23</v>
+      </c>
+      <c r="E231" s="10">
+        <v>38.5</v>
+      </c>
+      <c r="F231" s="10">
+        <v>-98</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>126</v>
+      </c>
+      <c r="B232" t="s">
+        <v>11</v>
+      </c>
+      <c r="E232" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>126</v>
+      </c>
+      <c r="B233" t="s">
+        <v>13</v>
+      </c>
+      <c r="C233" t="s">
+        <v>14</v>
+      </c>
+      <c r="D233" t="s">
+        <v>24</v>
+      </c>
+      <c r="E233">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>127</v>
+      </c>
+      <c r="B234" t="s">
+        <v>4</v>
+      </c>
+      <c r="D234" t="s">
+        <v>23</v>
+      </c>
+      <c r="E234" s="3">
+        <v>39.045752999999998</v>
+      </c>
+      <c r="F234" s="3">
+        <v>-76.641272999999998</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>127</v>
+      </c>
+      <c r="B235" t="s">
+        <v>11</v>
+      </c>
+      <c r="E235" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>127</v>
+      </c>
+      <c r="B236" t="s">
+        <v>13</v>
+      </c>
+      <c r="C236" t="s">
+        <v>14</v>
+      </c>
+      <c r="D236" t="s">
+        <v>24</v>
+      </c>
+      <c r="E236">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>128</v>
+      </c>
+      <c r="B237" t="s">
+        <v>4</v>
+      </c>
+      <c r="D237" t="s">
+        <v>23</v>
+      </c>
+      <c r="E237" s="3">
+        <v>36.778258999999998</v>
+      </c>
+      <c r="F237" s="3">
+        <v>-119.417931</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>128</v>
+      </c>
+      <c r="B238" t="s">
+        <v>11</v>
+      </c>
+      <c r="E238" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>128</v>
+      </c>
+      <c r="B239" t="s">
+        <v>13</v>
+      </c>
+      <c r="C239" t="s">
+        <v>14</v>
+      </c>
+      <c r="D239" t="s">
+        <v>24</v>
+      </c>
+      <c r="E239">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>129</v>
+      </c>
+      <c r="B240" t="s">
+        <v>4</v>
+      </c>
+      <c r="D240" t="s">
+        <v>23</v>
+      </c>
+      <c r="E240" s="3">
+        <v>40.367474000000001</v>
+      </c>
+      <c r="F240" s="3">
+        <v>-82.996216000000004</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>129</v>
+      </c>
+      <c r="B241" t="s">
+        <v>11</v>
+      </c>
+      <c r="E241" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>129</v>
+      </c>
+      <c r="B242" t="s">
+        <v>13</v>
+      </c>
+      <c r="C242" t="s">
+        <v>14</v>
+      </c>
+      <c r="D242" t="s">
+        <v>24</v>
+      </c>
+      <c r="E242">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>130</v>
+      </c>
+      <c r="B243" t="s">
+        <v>4</v>
+      </c>
+      <c r="D243" t="s">
+        <v>23</v>
+      </c>
+      <c r="E243" s="3">
+        <v>41.203322999999997</v>
+      </c>
+      <c r="F243" s="3">
+        <v>-77.194526999999994</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>130</v>
+      </c>
+      <c r="B244" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>130</v>
+      </c>
+      <c r="B245" t="s">
+        <v>13</v>
+      </c>
+      <c r="C245" t="s">
+        <v>14</v>
+      </c>
+      <c r="D245" t="s">
+        <v>24</v>
+      </c>
+      <c r="E245">
+        <v>71.23</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>133</v>
+      </c>
+      <c r="B246" t="s">
+        <v>4</v>
+      </c>
+      <c r="D246" t="s">
+        <v>23</v>
+      </c>
+      <c r="E246" s="10">
+        <v>31</v>
+      </c>
+      <c r="F246" s="10">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>133</v>
+      </c>
+      <c r="B247" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>133</v>
+      </c>
+      <c r="B248" t="s">
+        <v>13</v>
+      </c>
+      <c r="C248" t="s">
+        <v>14</v>
+      </c>
+      <c r="D248" t="s">
+        <v>24</v>
+      </c>
+      <c r="E248">
+        <v>284.93</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
         <v>15</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B250" t="s">
         <v>16</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C250" t="s">
         <v>25</v>
       </c>
-      <c r="E154">
+      <c r="E250">
         <v>0.997</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
         <v>15</v>
       </c>
-      <c r="B155" t="s">
-        <v>11</v>
-      </c>
-      <c r="E155" t="s">
+      <c r="B251" t="s">
+        <v>11</v>
+      </c>
+      <c r="E251" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
         <v>15</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B252" t="s">
         <v>26</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D252" t="s">
         <v>27</v>
       </c>
-      <c r="E156">
+      <c r="E252">
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
         <v>21</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B253" t="s">
         <v>12</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D253" t="s">
         <v>17</v>
       </c>
-      <c r="E157">
+      <c r="E253">
         <v>23.45</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
         <v>21</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B254" t="s">
         <v>12</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D254" t="s">
         <v>18</v>
       </c>
-      <c r="E158">
+      <c r="E254">
         <v>0.42370000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
         <v>21</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B255" t="s">
         <v>12</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D255" t="s">
         <v>19</v>
       </c>
-      <c r="E159">
+      <c r="E255">
         <v>0.50549999999999995</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
         <v>21</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B256" t="s">
         <v>12</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D256" t="s">
         <v>20</v>
       </c>
-      <c r="E160">
+      <c r="E256">
         <v>0.27110000000000001</v>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E182" s="1"/>
-    </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E183" s="1"/>
-    </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E184" s="1"/>
-    </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E185" s="1"/>
+    <row r="278" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E278" s="1"/>
+    </row>
+    <row r="279" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E279" s="1"/>
+    </row>
+    <row r="280" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E280" s="1"/>
+    </row>
+    <row r="281" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E281" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Added solar noise, modified values of capacity in META
</commit_message>
<xml_diff>
--- a/META.xlsx
+++ b/META.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0469B8B-C4E6-4AFA-A857-03D2CD6CC983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F55F22-99D5-47DE-9017-A77C2D43004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1524" yWindow="792" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="3792" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="144">
   <si>
     <t>Variable</t>
   </si>
@@ -433,6 +433,36 @@
   </si>
   <si>
     <t>c49</t>
+  </si>
+  <si>
+    <t>solar_1</t>
+  </si>
+  <si>
+    <t>solar_2</t>
+  </si>
+  <si>
+    <t>solar_3</t>
+  </si>
+  <si>
+    <t>solar_4</t>
+  </si>
+  <si>
+    <t>solar_5</t>
+  </si>
+  <si>
+    <t>solar_6</t>
+  </si>
+  <si>
+    <t>solar_7</t>
+  </si>
+  <si>
+    <t>solar_8</t>
+  </si>
+  <si>
+    <t>solar_9</t>
+  </si>
+  <si>
+    <t>solar_10</t>
   </si>
 </sst>
 </file>
@@ -440,7 +470,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -460,12 +490,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -489,18 +521,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="E248" sqref="E248"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -856,8 +885,8 @@
       <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1">
-        <v>250</v>
+      <c r="E4" s="7">
+        <v>219.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -885,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -902,7 +931,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -930,7 +959,7 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -947,7 +976,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -975,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -992,7 +1021,7 @@
         <v>24</v>
       </c>
       <c r="E13" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1020,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,7 +1066,7 @@
         <v>24</v>
       </c>
       <c r="E16" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1065,7 +1094,7 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1082,7 +1111,7 @@
         <v>24</v>
       </c>
       <c r="E19" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1110,7 +1139,7 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1127,7 +1156,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1155,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1172,7 +1201,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1200,7 +1229,7 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1217,7 +1246,7 @@
         <v>24</v>
       </c>
       <c r="E28" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1245,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1262,7 +1291,7 @@
         <v>24</v>
       </c>
       <c r="E31" s="1">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1324,8 +1353,8 @@
       <c r="D37" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="1">
-        <v>75</v>
+      <c r="E37" s="7">
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1370,7 +1399,7 @@
         <v>24</v>
       </c>
       <c r="E40" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1415,7 +1444,7 @@
         <v>24</v>
       </c>
       <c r="E43" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1460,7 +1489,7 @@
         <v>24</v>
       </c>
       <c r="E46" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1505,7 +1534,7 @@
         <v>24</v>
       </c>
       <c r="E49" s="1">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1550,7 +1579,7 @@
         <v>24</v>
       </c>
       <c r="E52" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1595,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="E55" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1640,7 +1669,7 @@
         <v>24</v>
       </c>
       <c r="E58" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1685,7 +1714,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="1">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,7 +1759,7 @@
         <v>24</v>
       </c>
       <c r="E64" s="1">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1775,7 +1804,7 @@
         <v>24</v>
       </c>
       <c r="E67" s="1">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1820,7 +1849,7 @@
         <v>24</v>
       </c>
       <c r="E70" s="1">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -1865,7 +1894,7 @@
         <v>24</v>
       </c>
       <c r="E73" s="1">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1923,10 +1952,10 @@
       <c r="D77" t="s">
         <v>23</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="2">
         <v>36.778258999999998</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="2">
         <v>-119.417931</v>
       </c>
     </row>
@@ -1968,10 +1997,10 @@
       <c r="D80" t="s">
         <v>23</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="4">
         <v>44</v>
       </c>
-      <c r="F80" s="5">
+      <c r="F80" s="4">
         <v>-120.5</v>
       </c>
     </row>
@@ -2013,10 +2042,10 @@
       <c r="D83" t="s">
         <v>23</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="4">
         <v>43</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="4">
         <v>-75</v>
       </c>
     </row>
@@ -2058,10 +2087,10 @@
       <c r="D86" t="s">
         <v>23</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86" s="4">
         <v>32.31823</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F86" s="2">
         <v>-86.902298000000002</v>
       </c>
     </row>
@@ -2103,10 +2132,10 @@
       <c r="D89" t="s">
         <v>23</v>
       </c>
-      <c r="E89" s="9">
+      <c r="E89" s="5">
         <v>21.167635000000001</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="5">
         <v>-105.22829400000001</v>
       </c>
     </row>
@@ -4045,7 +4074,7 @@
       <c r="D225" t="s">
         <v>23</v>
       </c>
-      <c r="E225" s="10">
+      <c r="E225" s="6">
         <v>30.391829999999999</v>
       </c>
       <c r="F225" s="3">
@@ -4090,10 +4119,10 @@
       <c r="D228" t="s">
         <v>23</v>
       </c>
-      <c r="E228" s="10">
+      <c r="E228" s="6">
         <v>31</v>
       </c>
-      <c r="F228" s="10">
+      <c r="F228" s="6">
         <v>-100</v>
       </c>
     </row>
@@ -4135,10 +4164,10 @@
       <c r="D231" t="s">
         <v>23</v>
       </c>
-      <c r="E231" s="10">
+      <c r="E231" s="6">
         <v>38.5</v>
       </c>
-      <c r="F231" s="10">
+      <c r="F231" s="6">
         <v>-98</v>
       </c>
     </row>
@@ -4360,10 +4389,10 @@
       <c r="D246" t="s">
         <v>23</v>
       </c>
-      <c r="E246" s="10">
+      <c r="E246" s="6">
         <v>31</v>
       </c>
-      <c r="F246" s="10">
+      <c r="F246" s="6">
         <v>-100</v>
       </c>
     </row>

</xml_diff>